<commit_message>
1. Added file 'energystorage.m', which gives all energystorage data, including cost 2. Modified distregions.m to give data in all columns and not just diagonally 3. WIP: Transmission losses
</commit_message>
<xml_diff>
--- a/storage/storageoptions.xlsx
+++ b/storage/storageoptions.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>StorageType</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Hydro</t>
   </si>
   <si>
-    <t>RoundTripEfficiency</t>
-  </si>
-  <si>
     <t>Crate</t>
   </si>
   <si>
@@ -54,6 +51,15 @@
   </si>
   <si>
     <t>inf</t>
+  </si>
+  <si>
+    <t>Limits</t>
+  </si>
+  <si>
+    <t>RampTime(Hrs)</t>
+  </si>
+  <si>
+    <t>AvgEfficiency</t>
   </si>
 </sst>
 </file>
@@ -368,20 +374,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -389,16 +398,22 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -409,13 +424,19 @@
         <v>0.9</v>
       </c>
       <c r="D2">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>0.25</v>
+      </c>
+      <c r="G2">
+        <v>0.7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -429,24 +450,36 @@
         <v>0.1</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>0.25</v>
+      </c>
+      <c r="G3">
+        <v>0.8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>50000</v>
+        <v>5000</v>
       </c>
       <c r="C4">
         <v>0.8</v>
       </c>
       <c r="D4">
-        <v>5.0000000000000001E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="E4">
         <v>10000000</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>